<commit_message>
feat: update new rawdata
</commit_message>
<xml_diff>
--- a/metadata/sample-metadata.xlsx
+++ b/metadata/sample-metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\Documents\TCL38\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F178159F-2375-4664-9180-58C828FA64A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F2C7D61-6602-488B-98CA-C9C373E25FAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{77D6BAED-54B8-4635-8275-C86F07E38C05}"/>
+    <workbookView xWindow="54600" yWindow="0" windowWidth="25800" windowHeight="21150" xr2:uid="{77D6BAED-54B8-4635-8275-C86F07E38C05}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="58">
   <si>
     <t>DEL</t>
   </si>
@@ -122,9 +122,6 @@
     <t>Loucy</t>
   </si>
   <si>
-    <t>PEER</t>
-  </si>
-  <si>
     <t>Jurkat</t>
   </si>
   <si>
@@ -197,100 +194,22 @@
     <t>Cell.Line</t>
   </si>
   <si>
-    <t>DL40</t>
-  </si>
-  <si>
-    <t>L82</t>
-  </si>
-  <si>
-    <t>SUDHL1</t>
-  </si>
-  <si>
-    <t>SUPM2</t>
-  </si>
-  <si>
-    <t>TLBR1</t>
-  </si>
-  <si>
-    <t>TLBR2</t>
-  </si>
-  <si>
-    <t>DERL2</t>
-  </si>
-  <si>
-    <t>DERL7</t>
-  </si>
-  <si>
-    <t>KARPAS299</t>
-  </si>
-  <si>
-    <t>KHYG1</t>
-  </si>
-  <si>
-    <t>NK92</t>
-  </si>
-  <si>
-    <t>SNK6</t>
-  </si>
-  <si>
-    <t>MOTN1</t>
-  </si>
-  <si>
-    <t>SMZ1</t>
-  </si>
-  <si>
-    <t>DND41</t>
-  </si>
-  <si>
-    <t>SUPT11</t>
-  </si>
-  <si>
-    <t>CCRFHSB2</t>
-  </si>
-  <si>
-    <t>KOPTK1</t>
-  </si>
-  <si>
-    <t>MOLT4</t>
-  </si>
-  <si>
-    <t>MAC1</t>
-  </si>
-  <si>
-    <t>MAC2A</t>
-  </si>
-  <si>
-    <t>HUT78</t>
-  </si>
-  <si>
-    <t>MYLA</t>
-  </si>
-  <si>
-    <t>KARPAS384</t>
-  </si>
-  <si>
-    <t>OCILY132</t>
-  </si>
-  <si>
-    <t>SEAX</t>
-  </si>
-  <si>
-    <t>NKYS</t>
-  </si>
-  <si>
-    <t>LOUCY</t>
-  </si>
-  <si>
-    <t>JURKAT</t>
-  </si>
-  <si>
-    <t>ALLSIL</t>
-  </si>
-  <si>
-    <t>SUPT13</t>
-  </si>
-  <si>
     <t>sampleid</t>
+  </si>
+  <si>
+    <t>HUT-78</t>
+  </si>
+  <si>
+    <t>Karpas 299</t>
+  </si>
+  <si>
+    <t>Karpas 384</t>
+  </si>
+  <si>
+    <t>Peer</t>
+  </si>
+  <si>
+    <t>SUP-T11</t>
   </si>
 </sst>
 </file>
@@ -665,7 +584,7 @@
   <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -675,33 +594,33 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>84</v>
+        <v>52</v>
       </c>
       <c r="B1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E2" t="s">
         <v>47</v>
@@ -709,16 +628,16 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>30</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E3" t="s">
         <v>47</v>
@@ -726,33 +645,33 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>61</v>
+        <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>50</v>
       </c>
       <c r="C5" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="D5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E5" t="s">
         <v>47</v>
@@ -760,16 +679,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>55</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="D6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E6" t="s">
         <v>47</v>
@@ -777,50 +696,50 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>72</v>
+        <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>73</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>77</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C9" t="s">
         <v>35</v>
       </c>
       <c r="D9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E9" t="s">
         <v>48</v>
@@ -828,33 +747,33 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>56</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C10" t="s">
         <v>35</v>
       </c>
       <c r="D10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C11" t="s">
         <v>35</v>
       </c>
       <c r="D11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E11" t="s">
         <v>48</v>
@@ -862,16 +781,16 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>58</v>
+        <v>28</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D12" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E12" t="s">
         <v>48</v>
@@ -879,152 +798,152 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>78</v>
+        <v>54</v>
       </c>
       <c r="B13" t="s">
-        <v>50</v>
+        <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>55</v>
       </c>
       <c r="B14" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E14" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>74</v>
+        <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C15" t="s">
         <v>36</v>
       </c>
       <c r="D15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E15" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="B16" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="C16" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D16" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>75</v>
+        <v>3</v>
       </c>
       <c r="B17" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="C17" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E17" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>59</v>
+        <v>27</v>
       </c>
       <c r="B18" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
       <c r="C18" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D18" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E18" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>60</v>
+        <v>5</v>
       </c>
       <c r="B19" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C19" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>76</v>
+        <v>6</v>
       </c>
       <c r="B20" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C20" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>62</v>
+        <v>32</v>
       </c>
       <c r="B21" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="C21" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D21" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E21" t="s">
         <v>47</v>
@@ -1032,16 +951,16 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B22" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="C22" t="s">
         <v>37</v>
       </c>
       <c r="D22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E22" t="s">
         <v>47</v>
@@ -1049,50 +968,50 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>63</v>
+        <v>18</v>
       </c>
       <c r="B23" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E23" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>79</v>
+        <v>14</v>
       </c>
       <c r="B24" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C24" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E24" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B25" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E25" t="s">
         <v>48</v>
@@ -1100,115 +1019,115 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>64</v>
+        <v>20</v>
       </c>
       <c r="B26" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C26" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D26" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E26" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B27" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E27" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>65</v>
+        <v>7</v>
       </c>
       <c r="B28" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="C28" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D28" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E28" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="B29" t="s">
-        <v>25</v>
+        <v>56</v>
       </c>
       <c r="C29" t="s">
         <v>39</v>
       </c>
       <c r="D29" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E29" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="B30" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="C30" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D30" t="s">
         <v>44</v>
       </c>
       <c r="E30" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>80</v>
+        <v>25</v>
       </c>
       <c r="B31" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C31" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D31" t="s">
         <v>44</v>
       </c>
       <c r="E31" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B32" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C32" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D32" t="s">
         <v>44</v>
@@ -1219,67 +1138,67 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>81</v>
+        <v>4</v>
       </c>
       <c r="B33" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="C33" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D33" t="s">
         <v>44</v>
       </c>
       <c r="E33" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>83</v>
+        <v>8</v>
       </c>
       <c r="B34" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34" t="s">
         <v>34</v>
       </c>
-      <c r="C34" t="s">
-        <v>40</v>
-      </c>
       <c r="D34" t="s">
         <v>44</v>
       </c>
       <c r="E34" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>82</v>
+        <v>57</v>
       </c>
       <c r="B35" t="s">
-        <v>30</v>
+        <v>57</v>
       </c>
       <c r="C35" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D35" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E35" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>69</v>
+        <v>33</v>
       </c>
       <c r="B36" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C36" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D36" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E36" t="s">
         <v>48</v>
@@ -1287,56 +1206,59 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="B37" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="C37" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D37" t="s">
         <v>44</v>
       </c>
       <c r="E37" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>71</v>
+        <v>10</v>
       </c>
       <c r="B38" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="C38" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D38" t="s">
         <v>44</v>
       </c>
       <c r="E38" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>68</v>
+        <v>23</v>
       </c>
       <c r="B39" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="C39" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D39" t="s">
         <v>44</v>
       </c>
       <c r="E39" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E39">
+    <sortCondition ref="A3:A39"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>